<commit_message>
Updated reconciliation results in test data
Added reconciliation status and remarks
</commit_message>
<xml_diff>
--- a/test-data/Data_Reconciliation_Test_Data.xlsx
+++ b/test-data/Data_Reconciliation_Test_Data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chandraiahgobburu/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558F95B4-70B6-9642-8BA8-157AEA4018BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48A7DC6-FD89-C84D-A5C9-4AF0885EB52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8780" yWindow="4100" windowWidth="27640" windowHeight="16940" xr2:uid="{BB67C954-6EDA-CD4A-96E5-2D44452A2AB4}"/>
+    <workbookView xWindow="8780" yWindow="4100" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{BB67C954-6EDA-CD4A-96E5-2D44452A2AB4}"/>
   </bookViews>
   <sheets>
     <sheet name="SourceA_Bank_Transactions" sheetId="1" r:id="rId1"/>
     <sheet name="SourceB_Ledger_Transactions" sheetId="2" r:id="rId2"/>
+    <sheet name="Reconciliation_Result" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="72">
   <si>
     <t>Transaction_ID</t>
   </si>
@@ -217,13 +218,49 @@
   </si>
   <si>
     <t>ACC1022</t>
+  </si>
+  <si>
+    <t>SourceA_Amount</t>
+  </si>
+  <si>
+    <t>SourceB_Amount</t>
+  </si>
+  <si>
+    <t>Reconciliation_Status</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>MATCHED</t>
+  </si>
+  <si>
+    <t>AMOUNT_MISMATCH</t>
+  </si>
+  <si>
+    <t>MISSING_IN_LEDGER</t>
+  </si>
+  <si>
+    <t>EXTRA_IN_LEDGER</t>
+  </si>
+  <si>
+    <t>Transaction matched successfully between Source A and Source B</t>
+  </si>
+  <si>
+    <t>Amount mismatch between Source A and Source B</t>
+  </si>
+  <si>
+    <t>Transaction present in Source A but missing in Source B (Ledger)</t>
+  </si>
+  <si>
+    <t>Transaction present in Source B (Ledger) but missing in Source A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -235,6 +272,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -269,6 +312,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -308,9 +354,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -325,12 +368,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A80FD9C-9B54-CF46-B2B4-9D8F40AB33E4}" name="Table1" displayName="Table1" ref="A1:H22" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A80FD9C-9B54-CF46-B2B4-9D8F40AB33E4}" name="Table1" displayName="Table1" ref="A1:H22" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:H22" xr:uid="{4A80FD9C-9B54-CF46-B2B4-9D8F40AB33E4}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{AE031BC7-F5B4-BD42-826F-214AA1E0F1BA}" name="Transaction_ID"/>
     <tableColumn id="2" xr3:uid="{4B06F2EC-286D-AC43-AB83-EB05D1F6E80B}" name="Account_Number"/>
-    <tableColumn id="3" xr3:uid="{C5A5232D-F74A-7146-AA0D-FC72DB3E5F90}" name="Transaction_Date" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{C5A5232D-F74A-7146-AA0D-FC72DB3E5F90}" name="Transaction_Date" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{B8887758-FA0B-7B4C-99A2-9BCCC4FDD2A9}" name="Amount"/>
     <tableColumn id="5" xr3:uid="{499A8EA6-6F55-0146-A7FE-D739F01A1BEF}" name="Currency"/>
     <tableColumn id="6" xr3:uid="{669B1F60-4526-B94E-B037-FC26F182545F}" name="Transaction_Type"/>
@@ -342,17 +385,33 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6617F17F-9005-D44D-B8F3-8C486D4A61BB}" name="Table2" displayName="Table2" ref="A1:H21" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6617F17F-9005-D44D-B8F3-8C486D4A61BB}" name="Table2" displayName="Table2" ref="A1:H21" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:H21" xr:uid="{6617F17F-9005-D44D-B8F3-8C486D4A61BB}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{75BFA197-FC59-6D42-8160-F4F3514DC27A}" name="Transaction_ID"/>
     <tableColumn id="2" xr3:uid="{18514DAC-4EA5-EA4B-B68A-A8B907894AE7}" name="Account_Number"/>
-    <tableColumn id="3" xr3:uid="{2E9641DE-9120-4343-AE2C-888274527359}" name="Transaction_Date" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{2E9641DE-9120-4343-AE2C-888274527359}" name="Transaction_Date" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{58F5E60D-2804-8A4C-A3BC-C9DAFF104D12}" name="Amount"/>
     <tableColumn id="5" xr3:uid="{5935EA3C-16C0-5F41-9408-C7D5B4ED227A}" name="Currency"/>
     <tableColumn id="6" xr3:uid="{A033572B-F202-3540-A662-65153687A406}" name="Transaction_Type"/>
     <tableColumn id="7" xr3:uid="{678FC4F2-6427-0440-8F62-CE2D4A28349B}" name="Source_System"/>
     <tableColumn id="8" xr3:uid="{29E0A0F0-1464-364B-9926-BD025E2DAEB3}" name="Status"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D696BD5A-A455-6443-A88F-D740EB66797F}" name="Table3" displayName="Table3" ref="A1:G8" totalsRowShown="0">
+  <autoFilter ref="A1:G8" xr:uid="{D696BD5A-A455-6443-A88F-D740EB66797F}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{63F168AE-7715-8D4F-A5F3-F2878423AB9D}" name="Transaction_ID"/>
+    <tableColumn id="2" xr3:uid="{A6B404D0-B42A-7046-8F98-ACC4DDE10A01}" name="Account_Number"/>
+    <tableColumn id="3" xr3:uid="{778A0223-BE46-E142-9FD1-6DD6C531FD7A}" name="SourceA_Amount"/>
+    <tableColumn id="4" xr3:uid="{25AC8655-6071-434D-B9BD-53B961D7AA5F}" name="SourceB_Amount"/>
+    <tableColumn id="5" xr3:uid="{48D82831-2387-DA44-B1F6-AFAF978CE101}" name="Currency"/>
+    <tableColumn id="6" xr3:uid="{3D61BE05-4B0D-D34A-A9BC-39C6DCE5A1C5}" name="Reconciliation_Status"/>
+    <tableColumn id="7" xr3:uid="{8738B3AA-8F79-D346-9132-6B32D5F5A2FA}" name="Remarks"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -677,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F297C89-0DC1-0A40-BBFD-EA4601E51CA4}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1250,7 +1309,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="B20" sqref="B20:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1815,4 +1874,205 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ACA877E-0C95-2C4E-B5FA-B3EF1B2081A6}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="3" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="21.5" customWidth="1"/>
+    <col min="7" max="7" width="77" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>500</v>
+      </c>
+      <c r="D2">
+        <v>500</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>400</v>
+      </c>
+      <c r="D3">
+        <v>450</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4">
+        <v>750</v>
+      </c>
+      <c r="D4">
+        <v>700</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5">
+        <v>350</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <v>500</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7">
+        <v>400</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8">
+        <v>900</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Test cases, defect log for reconciliation data issues
</commit_message>
<xml_diff>
--- a/test-data/Data_Reconciliation_Test_Data.xlsx
+++ b/test-data/Data_Reconciliation_Test_Data.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chandraiahgobburu/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48A7DC6-FD89-C84D-A5C9-4AF0885EB52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E5B9F6-335D-8C4C-9CED-F32F55610834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8780" yWindow="4100" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{BB67C954-6EDA-CD4A-96E5-2D44452A2AB4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="44800" windowHeight="24700" activeTab="4" xr2:uid="{BB67C954-6EDA-CD4A-96E5-2D44452A2AB4}"/>
   </bookViews>
   <sheets>
     <sheet name="SourceA_Bank_Transactions" sheetId="1" r:id="rId1"/>
     <sheet name="SourceB_Ledger_Transactions" sheetId="2" r:id="rId2"/>
     <sheet name="Reconciliation_Result" sheetId="4" r:id="rId3"/>
+    <sheet name="Test_Cases" sheetId="5" r:id="rId4"/>
+    <sheet name="Defect_Log" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="184">
   <si>
     <t>Transaction_ID</t>
   </si>
@@ -238,9 +240,6 @@
     <t>AMOUNT_MISMATCH</t>
   </si>
   <si>
-    <t>MISSING_IN_LEDGER</t>
-  </si>
-  <si>
     <t>EXTRA_IN_LEDGER</t>
   </si>
   <si>
@@ -250,17 +249,356 @@
     <t>Amount mismatch between Source A and Source B</t>
   </si>
   <si>
-    <t>Transaction present in Source A but missing in Source B (Ledger)</t>
-  </si>
-  <si>
     <t>Transaction present in Source B (Ledger) but missing in Source A</t>
+  </si>
+  <si>
+    <t>Test_Case_ID</t>
+  </si>
+  <si>
+    <t>Test_Scenario_ID</t>
+  </si>
+  <si>
+    <t>Test_Case_Description</t>
+  </si>
+  <si>
+    <t>SourceA_Condition</t>
+  </si>
+  <si>
+    <t>SourceB_Condition</t>
+  </si>
+  <si>
+    <t>Expected_Result</t>
+  </si>
+  <si>
+    <t>Actual_Result</t>
+  </si>
+  <si>
+    <t>TC_01</t>
+  </si>
+  <si>
+    <t>TS_01</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>TC_03</t>
+  </si>
+  <si>
+    <t>TC_04</t>
+  </si>
+  <si>
+    <t>TC_05</t>
+  </si>
+  <si>
+    <t>TC_06</t>
+  </si>
+  <si>
+    <t>TS_02</t>
+  </si>
+  <si>
+    <t>TS_03</t>
+  </si>
+  <si>
+    <t>TS_04</t>
+  </si>
+  <si>
+    <t>Transaction excluded from reconciliation</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Validate matched transaction TXN001</t>
+  </si>
+  <si>
+    <t>TXN001 exists with Status = PROCESSED and Amount = 500</t>
+  </si>
+  <si>
+    <t>TXN001 exists with Status = POSTED and Amount = 500</t>
+  </si>
+  <si>
+    <t>Transaction flagged as MATCHED</t>
+  </si>
+  <si>
+    <t>TXN001 flagged as MATCHED</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Validate matched transaction TXN005</t>
+  </si>
+  <si>
+    <t>TXN005 exists with Status = PROCESSED and Amount = 950</t>
+  </si>
+  <si>
+    <t>TXN005 exists with Status = POSTED and Amount = 950</t>
+  </si>
+  <si>
+    <t>TXN005 flagged as MATCHED</t>
+  </si>
+  <si>
+    <t>Validate amount mismatch for TXN006</t>
+  </si>
+  <si>
+    <t>TXN006 exists with Status = PROCESSED and Amount = 400</t>
+  </si>
+  <si>
+    <t>TXN006 exists with Status = POSTED and Amount = 450</t>
+  </si>
+  <si>
+    <t>Transaction flagged as AMOUNT_MISMATCH</t>
+  </si>
+  <si>
+    <t>TXN006 flagged as AMOUNT_MISMATCH</t>
+  </si>
+  <si>
+    <t>Validate amount mismatch for TXN015</t>
+  </si>
+  <si>
+    <t>TXN015 exists with Status = PROCESSED and Amount = 750</t>
+  </si>
+  <si>
+    <t>TXN015 exists with Status = POSTED and Amount = 700</t>
+  </si>
+  <si>
+    <t>TXN015 flagged as AMOUNT_MISMATCH</t>
+  </si>
+  <si>
+    <t>Validate missing ledger entry for TXN016</t>
+  </si>
+  <si>
+    <t>TXN016 exists with Status = FAILED</t>
+  </si>
+  <si>
+    <t>No matching Transaction_ID exists</t>
+  </si>
+  <si>
+    <t>TXN016 excluded from reconciliation</t>
+  </si>
+  <si>
+    <t>FAILED transactions correctly excluded</t>
+  </si>
+  <si>
+    <t>Validate missing ledger entry for TXN017</t>
+  </si>
+  <si>
+    <t>TXN017 exists with Status = FAILED</t>
+  </si>
+  <si>
+    <t>TXN017 excluded from reconciliation</t>
+  </si>
+  <si>
+    <t>TC_07</t>
+  </si>
+  <si>
+    <t>Validate missing ledger for PROCESSED TXN018</t>
+  </si>
+  <si>
+    <t>TXN018 exists with Status = PROCESSED</t>
+  </si>
+  <si>
+    <t>TXN018 exists</t>
+  </si>
+  <si>
+    <t>Transaction reconciled</t>
+  </si>
+  <si>
+    <t>TXN018 reconciled</t>
+  </si>
+  <si>
+    <t>Valid PROCESSED transaction found in ledger</t>
+  </si>
+  <si>
+    <t>TC_08</t>
+  </si>
+  <si>
+    <t>Validate extra ledger record TXN021</t>
+  </si>
+  <si>
+    <t>TXN021 exists with Status = POSTED</t>
+  </si>
+  <si>
+    <t>Transaction flagged as EXTRA_IN_LEDGER</t>
+  </si>
+  <si>
+    <t>TXN021 flagged as EXTRA_IN_LEDGER</t>
+  </si>
+  <si>
+    <t>Ledger entry found without Source A transaction</t>
+  </si>
+  <si>
+    <t>TC_09</t>
+  </si>
+  <si>
+    <t>Validate extra ledger record TXN022</t>
+  </si>
+  <si>
+    <t>TXN022 exists with Status = POSTED</t>
+  </si>
+  <si>
+    <t>TXN022 flagged as EXTRA_IN_LEDGER</t>
+  </si>
+  <si>
+    <t>TC_10</t>
+  </si>
+  <si>
+    <t>TS_07</t>
+  </si>
+  <si>
+    <t>Validate transaction type mapping</t>
+  </si>
+  <si>
+    <t>Source A Transaction_Type = DEBIT</t>
+  </si>
+  <si>
+    <t>Source B Transaction_Type = CREDIT</t>
+  </si>
+  <si>
+    <t>Debit mapped to Credit correctly</t>
+  </si>
+  <si>
+    <t>Transaction type mapping validated</t>
+  </si>
+  <si>
+    <t>TC_11</t>
+  </si>
+  <si>
+    <t>TS_06</t>
+  </si>
+  <si>
+    <t>Validate currency consistency</t>
+  </si>
+  <si>
+    <t>Currency = USD in Source A</t>
+  </si>
+  <si>
+    <t>Currency = USD in Source B</t>
+  </si>
+  <si>
+    <t>Currency matches</t>
+  </si>
+  <si>
+    <t>Currency consistent across systems</t>
+  </si>
+  <si>
+    <t>TC_12</t>
+  </si>
+  <si>
+    <t>TS_08</t>
+  </si>
+  <si>
+    <t>Validate reconciliation summary counts</t>
+  </si>
+  <si>
+    <t>18 PROCESSED transactions</t>
+  </si>
+  <si>
+    <t>Ledger contains 20 records</t>
+  </si>
+  <si>
+    <t>Correct counts displayed</t>
+  </si>
+  <si>
+    <t>Counts validated correctly</t>
+  </si>
+  <si>
+    <t>Reconciliation summary accurate</t>
+  </si>
+  <si>
+    <t>Defect_ID</t>
+  </si>
+  <si>
+    <t>Defect_Title</t>
+  </si>
+  <si>
+    <t>Defect_Type</t>
+  </si>
+  <si>
+    <t>Related_TestCase</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Identified_By</t>
+  </si>
+  <si>
+    <t>DEF_001</t>
+  </si>
+  <si>
+    <t>Amount mismatch between Source A and Ledger</t>
+  </si>
+  <si>
+    <t>Data Defect</t>
+  </si>
+  <si>
+    <t>Amounts should match between Source A and Source B</t>
+  </si>
+  <si>
+    <t>Source A = 400, Source B = 450</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Requires investigation by data/ops team</t>
+  </si>
+  <si>
+    <t>DEF_002</t>
+  </si>
+  <si>
+    <t>Source A = 750, Source B = 700</t>
+  </si>
+  <si>
+    <t>Possible posting or transformation issue</t>
+  </si>
+  <si>
+    <t>DEF_003</t>
+  </si>
+  <si>
+    <t>Transaction missing in Source A</t>
+  </si>
+  <si>
+    <t>Transaction should exist in both sources</t>
+  </si>
+  <si>
+    <t>Present only in Source B</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>Ledger-only entry found</t>
+  </si>
+  <si>
+    <t>DEF_004</t>
+  </si>
+  <si>
+    <t>Requires source system validation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -278,6 +616,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -303,15 +648,70 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
@@ -368,12 +768,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A80FD9C-9B54-CF46-B2B4-9D8F40AB33E4}" name="Table1" displayName="Table1" ref="A1:H22" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:H22" xr:uid="{4A80FD9C-9B54-CF46-B2B4-9D8F40AB33E4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A80FD9C-9B54-CF46-B2B4-9D8F40AB33E4}" name="Table1" displayName="Table1" ref="A1:H21" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:H21" xr:uid="{4A80FD9C-9B54-CF46-B2B4-9D8F40AB33E4}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{AE031BC7-F5B4-BD42-826F-214AA1E0F1BA}" name="Transaction_ID"/>
     <tableColumn id="2" xr3:uid="{4B06F2EC-286D-AC43-AB83-EB05D1F6E80B}" name="Account_Number"/>
-    <tableColumn id="3" xr3:uid="{C5A5232D-F74A-7146-AA0D-FC72DB3E5F90}" name="Transaction_Date" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{C5A5232D-F74A-7146-AA0D-FC72DB3E5F90}" name="Transaction_Date" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{B8887758-FA0B-7B4C-99A2-9BCCC4FDD2A9}" name="Amount"/>
     <tableColumn id="5" xr3:uid="{499A8EA6-6F55-0146-A7FE-D739F01A1BEF}" name="Currency"/>
     <tableColumn id="6" xr3:uid="{669B1F60-4526-B94E-B037-FC26F182545F}" name="Transaction_Type"/>
@@ -385,12 +785,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6617F17F-9005-D44D-B8F3-8C486D4A61BB}" name="Table2" displayName="Table2" ref="A1:H21" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6617F17F-9005-D44D-B8F3-8C486D4A61BB}" name="Table2" displayName="Table2" ref="A1:H21" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:H21" xr:uid="{6617F17F-9005-D44D-B8F3-8C486D4A61BB}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{75BFA197-FC59-6D42-8160-F4F3514DC27A}" name="Transaction_ID"/>
     <tableColumn id="2" xr3:uid="{18514DAC-4EA5-EA4B-B68A-A8B907894AE7}" name="Account_Number"/>
-    <tableColumn id="3" xr3:uid="{2E9641DE-9120-4343-AE2C-888274527359}" name="Transaction_Date" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{2E9641DE-9120-4343-AE2C-888274527359}" name="Transaction_Date" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{58F5E60D-2804-8A4C-A3BC-C9DAFF104D12}" name="Amount"/>
     <tableColumn id="5" xr3:uid="{5935EA3C-16C0-5F41-9408-C7D5B4ED227A}" name="Currency"/>
     <tableColumn id="6" xr3:uid="{A033572B-F202-3540-A662-65153687A406}" name="Transaction_Type"/>
@@ -402,16 +802,55 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D696BD5A-A455-6443-A88F-D740EB66797F}" name="Table3" displayName="Table3" ref="A1:G8" totalsRowShown="0">
-  <autoFilter ref="A1:G8" xr:uid="{D696BD5A-A455-6443-A88F-D740EB66797F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{73FD3FB2-A9EA-7C4F-9A63-A731D8066ED4}" name="Table3" displayName="Table3" ref="A1:G21" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:G21" xr:uid="{73FD3FB2-A9EA-7C4F-9A63-A731D8066ED4}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{63F168AE-7715-8D4F-A5F3-F2878423AB9D}" name="Transaction_ID"/>
-    <tableColumn id="2" xr3:uid="{A6B404D0-B42A-7046-8F98-ACC4DDE10A01}" name="Account_Number"/>
-    <tableColumn id="3" xr3:uid="{778A0223-BE46-E142-9FD1-6DD6C531FD7A}" name="SourceA_Amount"/>
-    <tableColumn id="4" xr3:uid="{25AC8655-6071-434D-B9BD-53B961D7AA5F}" name="SourceB_Amount"/>
-    <tableColumn id="5" xr3:uid="{48D82831-2387-DA44-B1F6-AFAF978CE101}" name="Currency"/>
-    <tableColumn id="6" xr3:uid="{3D61BE05-4B0D-D34A-A9BC-39C6DCE5A1C5}" name="Reconciliation_Status"/>
-    <tableColumn id="7" xr3:uid="{8738B3AA-8F79-D346-9132-6B32D5F5A2FA}" name="Remarks"/>
+    <tableColumn id="1" xr3:uid="{161B3E8F-0135-974D-980A-F0D1876B311D}" name="Transaction_ID"/>
+    <tableColumn id="2" xr3:uid="{E7664E46-6706-E948-A547-6A99E29B19AA}" name="Account_Number"/>
+    <tableColumn id="3" xr3:uid="{A9C6BF6E-00AE-C64F-84C7-9D1F5536671F}" name="SourceA_Amount"/>
+    <tableColumn id="4" xr3:uid="{9DFBEBA3-5A23-004F-AAE5-F8FAEF83E80D}" name="SourceB_Amount"/>
+    <tableColumn id="5" xr3:uid="{C7B1B61E-A381-A44B-90E3-104F9D5D5F12}" name="Currency"/>
+    <tableColumn id="6" xr3:uid="{5D52D0E6-59C4-A944-9246-9F9644428907}" name="Reconciliation_Status"/>
+    <tableColumn id="7" xr3:uid="{6525756F-21B2-BA42-A909-5EC3708C8D5C}" name="Remarks"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2E027714-E37E-5C4F-B8E8-0C889A5ADB6B}" name="Table4" displayName="Table4" ref="A1:I13" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:I13" xr:uid="{2E027714-E37E-5C4F-B8E8-0C889A5ADB6B}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{7CF7A502-F33B-254F-BBC9-846172958840}" name="Test_Case_ID"/>
+    <tableColumn id="2" xr3:uid="{03EC8296-7D16-CC42-82FD-415DB88F8D05}" name="Test_Scenario_ID"/>
+    <tableColumn id="3" xr3:uid="{9264AF17-7428-5546-814A-7CE097CB9E2C}" name="Test_Case_Description"/>
+    <tableColumn id="4" xr3:uid="{546BF993-1944-334B-9634-DF6A2E02B2BA}" name="SourceA_Condition"/>
+    <tableColumn id="5" xr3:uid="{BBE14C31-D61A-7C4F-8538-E4A33D21A87F}" name="SourceB_Condition"/>
+    <tableColumn id="6" xr3:uid="{DC89FD1A-8A11-AD4A-80CB-936B8CE3E2DD}" name="Expected_Result"/>
+    <tableColumn id="7" xr3:uid="{BC0FADA6-63C9-2642-9225-3BFEA6983297}" name="Actual_Result"/>
+    <tableColumn id="8" xr3:uid="{1174861E-11E0-C641-8A64-46F59E5D6B27}" name="Status"/>
+    <tableColumn id="9" xr3:uid="{D92EFE34-A29B-C346-B18D-8932032E5603}" name="Remarks"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3BBE73AB-4EEE-204A-835B-3B6913DB6607}" name="Table5" displayName="Table5" ref="A1:L5" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:L5" xr:uid="{3BBE73AB-4EEE-204A-835B-3B6913DB6607}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{95A49FE6-7F0B-0F42-9FEC-903C1BC514D3}" name="Defect_ID"/>
+    <tableColumn id="2" xr3:uid="{80A25080-6EA4-0B49-A687-88A1FF6B9D04}" name="Defect_Title"/>
+    <tableColumn id="3" xr3:uid="{939E2B14-FBCC-2E4C-916A-CC97DED45D16}" name="Defect_Type"/>
+    <tableColumn id="4" xr3:uid="{8F2A221D-FD6A-174C-8E25-9FF0BE0E1861}" name="Related_TestCase"/>
+    <tableColumn id="5" xr3:uid="{0076E261-017E-2D4A-A4BB-D2C910759BA7}" name="Transaction_ID"/>
+    <tableColumn id="6" xr3:uid="{05C12A0F-648C-5742-8249-6725DA772B86}" name="Expected_Result"/>
+    <tableColumn id="7" xr3:uid="{DA3AF6AE-01A0-0F4B-A1CE-9A51A252BAAC}" name="Actual_Result"/>
+    <tableColumn id="8" xr3:uid="{D49CDF00-0C15-FF4D-8483-DC23929F215A}" name="Severity"/>
+    <tableColumn id="9" xr3:uid="{15EA852C-8E72-644F-9A03-715AA55E91AC}" name="Priority"/>
+    <tableColumn id="10" xr3:uid="{35DFC401-5CAF-2D4F-8337-179E7B7AD8E4}" name="Status"/>
+    <tableColumn id="11" xr3:uid="{9F46E550-BAC6-5547-A2B0-8A5052B2AE10}" name="Identified_By"/>
+    <tableColumn id="12" xr3:uid="{F8003E4A-36C2-EF4C-84A9-F203333CAD54}" name="Remarks"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -737,7 +1176,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:F18"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1878,10 +2317,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ACA877E-0C95-2C4E-B5FA-B3EF1B2081A6}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1895,25 +2334,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1937,135 +2376,444 @@
         <v>64</v>
       </c>
       <c r="G2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C3">
-        <v>400</v>
+        <v>1200</v>
       </c>
       <c r="D3">
-        <v>450</v>
+        <v>1200</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C4">
-        <v>750</v>
+        <v>300</v>
       </c>
       <c r="D4">
-        <v>700</v>
+        <v>300</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="C5">
-        <v>350</v>
+        <v>700</v>
+      </c>
+      <c r="D5">
+        <v>700</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="C6">
-        <v>500</v>
+        <v>950</v>
+      </c>
+      <c r="D6">
+        <v>950</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7">
+      <c r="A7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3">
         <v>400</v>
       </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G7" t="s">
-        <v>71</v>
+      <c r="D7" s="3">
+        <v>450</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>1100</v>
+      </c>
+      <c r="D8">
+        <v>1100</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <v>650</v>
+      </c>
+      <c r="D9">
+        <v>650</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <v>200</v>
+      </c>
+      <c r="D10">
+        <v>200</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11">
+        <v>800</v>
+      </c>
+      <c r="D11">
+        <v>800</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12">
+        <v>1500</v>
+      </c>
+      <c r="D12">
+        <v>1500</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13">
+        <v>100</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14">
+        <v>600</v>
+      </c>
+      <c r="D14">
+        <v>600</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15">
+        <v>900</v>
+      </c>
+      <c r="D15">
+        <v>900</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="3">
+        <v>750</v>
+      </c>
+      <c r="D16" s="3">
+        <v>700</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17">
+        <v>1200</v>
+      </c>
+      <c r="D17">
+        <v>1200</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18">
+        <v>650</v>
+      </c>
+      <c r="D18">
+        <v>650</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19">
+        <v>1000</v>
+      </c>
+      <c r="D19">
+        <v>1000</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="3">
+        <v>400</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B21" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8">
+      <c r="C21" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="3">
         <v>900</v>
       </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G8" t="s">
-        <v>71</v>
+      <c r="E21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2075,4 +2823,634 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC516FF-C67E-5148-83D6-CFFA9904EC1D}">
+  <dimension ref="A1:N13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" customWidth="1"/>
+    <col min="9" max="9" width="55.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" t="s">
+        <v>107</v>
+      </c>
+      <c r="H5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F6" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H6" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" t="s">
+        <v>121</v>
+      </c>
+      <c r="H8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" t="s">
+        <v>125</v>
+      </c>
+      <c r="F9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" t="s">
+        <v>127</v>
+      </c>
+      <c r="H9" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10" t="s">
+        <v>132</v>
+      </c>
+      <c r="H10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" t="s">
+        <v>136</v>
+      </c>
+      <c r="E11" t="s">
+        <v>137</v>
+      </c>
+      <c r="F11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G11" t="s">
+        <v>138</v>
+      </c>
+      <c r="H11" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" t="s">
+        <v>142</v>
+      </c>
+      <c r="D12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E12" t="s">
+        <v>144</v>
+      </c>
+      <c r="F12" t="s">
+        <v>145</v>
+      </c>
+      <c r="G12" t="s">
+        <v>145</v>
+      </c>
+      <c r="H12" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" t="s">
+        <v>146</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" t="s">
+        <v>148</v>
+      </c>
+      <c r="C13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" t="s">
+        <v>150</v>
+      </c>
+      <c r="E13" t="s">
+        <v>151</v>
+      </c>
+      <c r="F13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G13" t="s">
+        <v>153</v>
+      </c>
+      <c r="H13" t="s">
+        <v>94</v>
+      </c>
+      <c r="I13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33BC1C49-4B53-0B49-B876-000EAA30EC77}">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="41.5" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="47.1640625" customWidth="1"/>
+    <col min="7" max="8" width="39.5" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" customWidth="1"/>
+    <col min="12" max="12" width="53.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H2" t="s">
+        <v>167</v>
+      </c>
+      <c r="I2" t="s">
+        <v>168</v>
+      </c>
+      <c r="J2" t="s">
+        <v>169</v>
+      </c>
+      <c r="K2" t="s">
+        <v>170</v>
+      </c>
+      <c r="L2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G3" t="s">
+        <v>173</v>
+      </c>
+      <c r="H3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I3" t="s">
+        <v>168</v>
+      </c>
+      <c r="J3" t="s">
+        <v>169</v>
+      </c>
+      <c r="K3" t="s">
+        <v>170</v>
+      </c>
+      <c r="L3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G4" t="s">
+        <v>178</v>
+      </c>
+      <c r="H4" t="s">
+        <v>179</v>
+      </c>
+      <c r="I4" t="s">
+        <v>180</v>
+      </c>
+      <c r="J4" t="s">
+        <v>169</v>
+      </c>
+      <c r="K4" t="s">
+        <v>170</v>
+      </c>
+      <c r="L4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" t="s">
+        <v>177</v>
+      </c>
+      <c r="G5" t="s">
+        <v>178</v>
+      </c>
+      <c r="H5" t="s">
+        <v>179</v>
+      </c>
+      <c r="I5" t="s">
+        <v>180</v>
+      </c>
+      <c r="J5" t="s">
+        <v>169</v>
+      </c>
+      <c r="K5" t="s">
+        <v>170</v>
+      </c>
+      <c r="L5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Requirement Traceability Matrix (RTM)
</commit_message>
<xml_diff>
--- a/test-data/Data_Reconciliation_Test_Data.xlsx
+++ b/test-data/Data_Reconciliation_Test_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chandraiahgobburu/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E5B9F6-335D-8C4C-9CED-F32F55610834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB004997-62B7-2840-B6D9-BCC04412A062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="44800" windowHeight="24700" activeTab="4" xr2:uid="{BB67C954-6EDA-CD4A-96E5-2D44452A2AB4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="44800" windowHeight="24700" activeTab="5" xr2:uid="{BB67C954-6EDA-CD4A-96E5-2D44452A2AB4}"/>
   </bookViews>
   <sheets>
     <sheet name="SourceA_Bank_Transactions" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Reconciliation_Result" sheetId="4" r:id="rId3"/>
     <sheet name="Test_Cases" sheetId="5" r:id="rId4"/>
     <sheet name="Defect_Log" sheetId="6" r:id="rId5"/>
+    <sheet name="RTM" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="222">
   <si>
     <t>Transaction_ID</t>
   </si>
@@ -592,6 +593,120 @@
   </si>
   <si>
     <t>Requires source system validation</t>
+  </si>
+  <si>
+    <t>Requirement_ID</t>
+  </si>
+  <si>
+    <t>Requirement_Description</t>
+  </si>
+  <si>
+    <t>Reconciliation_Rule_ID</t>
+  </si>
+  <si>
+    <t>Test_Case_Status</t>
+  </si>
+  <si>
+    <t>RQ_01</t>
+  </si>
+  <si>
+    <t>Only PROCESSED transactions from Source A should be reconciled</t>
+  </si>
+  <si>
+    <t>RR_01</t>
+  </si>
+  <si>
+    <t>–</t>
+  </si>
+  <si>
+    <t>RQ_02</t>
+  </si>
+  <si>
+    <t>Transaction IDs must be unique across both sources</t>
+  </si>
+  <si>
+    <t>RR_02</t>
+  </si>
+  <si>
+    <t>No duplicate transaction IDs found</t>
+  </si>
+  <si>
+    <t>RQ_03</t>
+  </si>
+  <si>
+    <t>Eligible transactions must exist in both Source A and Ledger</t>
+  </si>
+  <si>
+    <t>RR_03</t>
+  </si>
+  <si>
+    <t>DEF_003, DEF_004</t>
+  </si>
+  <si>
+    <t>Extra ledger records identified</t>
+  </si>
+  <si>
+    <t>RQ_04</t>
+  </si>
+  <si>
+    <t>Transaction amount must match between Source A and Ledger</t>
+  </si>
+  <si>
+    <t>RR_04</t>
+  </si>
+  <si>
+    <t>DEF_001, DEF_002</t>
+  </si>
+  <si>
+    <t>Amount mismatches correctly flagged</t>
+  </si>
+  <si>
+    <t>RQ_05</t>
+  </si>
+  <si>
+    <t>Currency should be consistent across both sources</t>
+  </si>
+  <si>
+    <t>RR_05</t>
+  </si>
+  <si>
+    <t>Currency matched for all eligible records</t>
+  </si>
+  <si>
+    <t>RQ_06</t>
+  </si>
+  <si>
+    <t>FAILED or CANCELLED transactions must be excluded from reconciliation</t>
+  </si>
+  <si>
+    <t>RR_06</t>
+  </si>
+  <si>
+    <t>Exclusion validated successfully</t>
+  </si>
+  <si>
+    <t>RQ_07</t>
+  </si>
+  <si>
+    <t>Reconciliation results must classify records correctly</t>
+  </si>
+  <si>
+    <t>RR_07</t>
+  </si>
+  <si>
+    <t>MATCHED / MISMATCH / EXTRA identified</t>
+  </si>
+  <si>
+    <t>RQ_08</t>
+  </si>
+  <si>
+    <t>Reconciliation report must be generated for each batch cycle</t>
+  </si>
+  <si>
+    <t>RR_08</t>
+  </si>
+  <si>
+    <t>Report generated successfully</t>
   </si>
 </sst>
 </file>
@@ -657,7 +772,25 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -768,12 +901,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A80FD9C-9B54-CF46-B2B4-9D8F40AB33E4}" name="Table1" displayName="Table1" ref="A1:H21" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A80FD9C-9B54-CF46-B2B4-9D8F40AB33E4}" name="Table1" displayName="Table1" ref="A1:H21" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A1:H21" xr:uid="{4A80FD9C-9B54-CF46-B2B4-9D8F40AB33E4}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{AE031BC7-F5B4-BD42-826F-214AA1E0F1BA}" name="Transaction_ID"/>
     <tableColumn id="2" xr3:uid="{4B06F2EC-286D-AC43-AB83-EB05D1F6E80B}" name="Account_Number"/>
-    <tableColumn id="3" xr3:uid="{C5A5232D-F74A-7146-AA0D-FC72DB3E5F90}" name="Transaction_Date" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{C5A5232D-F74A-7146-AA0D-FC72DB3E5F90}" name="Transaction_Date" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{B8887758-FA0B-7B4C-99A2-9BCCC4FDD2A9}" name="Amount"/>
     <tableColumn id="5" xr3:uid="{499A8EA6-6F55-0146-A7FE-D739F01A1BEF}" name="Currency"/>
     <tableColumn id="6" xr3:uid="{669B1F60-4526-B94E-B037-FC26F182545F}" name="Transaction_Type"/>
@@ -785,12 +918,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6617F17F-9005-D44D-B8F3-8C486D4A61BB}" name="Table2" displayName="Table2" ref="A1:H21" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6617F17F-9005-D44D-B8F3-8C486D4A61BB}" name="Table2" displayName="Table2" ref="A1:H21" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:H21" xr:uid="{6617F17F-9005-D44D-B8F3-8C486D4A61BB}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{75BFA197-FC59-6D42-8160-F4F3514DC27A}" name="Transaction_ID"/>
     <tableColumn id="2" xr3:uid="{18514DAC-4EA5-EA4B-B68A-A8B907894AE7}" name="Account_Number"/>
-    <tableColumn id="3" xr3:uid="{2E9641DE-9120-4343-AE2C-888274527359}" name="Transaction_Date" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{2E9641DE-9120-4343-AE2C-888274527359}" name="Transaction_Date" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{58F5E60D-2804-8A4C-A3BC-C9DAFF104D12}" name="Amount"/>
     <tableColumn id="5" xr3:uid="{5935EA3C-16C0-5F41-9408-C7D5B4ED227A}" name="Currency"/>
     <tableColumn id="6" xr3:uid="{A033572B-F202-3540-A662-65153687A406}" name="Transaction_Type"/>
@@ -802,7 +935,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{73FD3FB2-A9EA-7C4F-9A63-A731D8066ED4}" name="Table3" displayName="Table3" ref="A1:G21" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{73FD3FB2-A9EA-7C4F-9A63-A731D8066ED4}" name="Table3" displayName="Table3" ref="A1:G21" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:G21" xr:uid="{73FD3FB2-A9EA-7C4F-9A63-A731D8066ED4}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{161B3E8F-0135-974D-980A-F0D1876B311D}" name="Transaction_ID"/>
@@ -818,7 +951,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2E027714-E37E-5C4F-B8E8-0C889A5ADB6B}" name="Table4" displayName="Table4" ref="A1:I13" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2E027714-E37E-5C4F-B8E8-0C889A5ADB6B}" name="Table4" displayName="Table4" ref="A1:I13" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:I13" xr:uid="{2E027714-E37E-5C4F-B8E8-0C889A5ADB6B}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{7CF7A502-F33B-254F-BBC9-846172958840}" name="Test_Case_ID"/>
@@ -836,7 +969,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3BBE73AB-4EEE-204A-835B-3B6913DB6607}" name="Table5" displayName="Table5" ref="A1:L5" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3BBE73AB-4EEE-204A-835B-3B6913DB6607}" name="Table5" displayName="Table5" ref="A1:L5" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:L5" xr:uid="{3BBE73AB-4EEE-204A-835B-3B6913DB6607}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{95A49FE6-7F0B-0F42-9FEC-903C1BC514D3}" name="Defect_ID"/>
@@ -851,6 +984,22 @@
     <tableColumn id="10" xr3:uid="{35DFC401-5CAF-2D4F-8337-179E7B7AD8E4}" name="Status"/>
     <tableColumn id="11" xr3:uid="{9F46E550-BAC6-5547-A2B0-8A5052B2AE10}" name="Identified_By"/>
     <tableColumn id="12" xr3:uid="{F8003E4A-36C2-EF4C-84A9-F203333CAD54}" name="Remarks"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{FDE24166-C836-BC4A-A0C4-7183E647291F}" name="Table6" displayName="Table6" ref="A1:G9" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:G9" xr:uid="{FDE24166-C836-BC4A-A0C4-7183E647291F}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{775F316E-642D-6143-8AD7-9F761339FDB2}" name="Requirement_ID"/>
+    <tableColumn id="2" xr3:uid="{1D3A06AD-EF70-2540-A66F-12FD790AB453}" name="Requirement_Description"/>
+    <tableColumn id="3" xr3:uid="{D8FFDD39-1E61-3B4A-9FF9-E20A06038C3C}" name="Reconciliation_Rule_ID"/>
+    <tableColumn id="4" xr3:uid="{B62B3A5E-3062-7F4B-9F71-845613157FF5}" name="Test_Case_ID"/>
+    <tableColumn id="5" xr3:uid="{F69CA593-9C58-964B-954C-186D6768A5DB}" name="Test_Case_Status"/>
+    <tableColumn id="6" xr3:uid="{1AEF1CFC-48F5-CB4D-A73A-311C9724FD14}" name="Defect_ID"/>
+    <tableColumn id="7" xr3:uid="{EB505D19-7251-ED45-A136-19A7F924C45B}" name="Remarks"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3239,7 +3388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33BC1C49-4B53-0B49-B876-000EAA30EC77}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -3453,4 +3602,238 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9553CAA1-73A9-2941-BFD7-E6027D8938B1}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="61.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" t="s">
+        <v>199</v>
+      </c>
+      <c r="G4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" t="s">
+        <v>204</v>
+      </c>
+      <c r="G5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C6" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" t="s">
+        <v>191</v>
+      </c>
+      <c r="G6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" t="s">
+        <v>191</v>
+      </c>
+      <c r="G7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C8" t="s">
+        <v>216</v>
+      </c>
+      <c r="D8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" t="s">
+        <v>191</v>
+      </c>
+      <c r="G8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>218</v>
+      </c>
+      <c r="B9" t="s">
+        <v>219</v>
+      </c>
+      <c r="C9" t="s">
+        <v>220</v>
+      </c>
+      <c r="D9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" t="s">
+        <v>191</v>
+      </c>
+      <c r="G9" t="s">
+        <v>221</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>